<commit_message>
Adding exception for code formatting
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/LinkedList_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB75874-1E58-6844-87AC-2627415675C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD937DBB-74CC-734C-8ECA-D73EBB3D3949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72000" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="74900" yWindow="500" windowWidth="32980" windowHeight="18000" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Classroom" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubric" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>AutoTest Setup</t>
   </si>
@@ -168,6 +169,15 @@
   </si>
   <si>
     <t>./LinkedList_AutoTest/AutoTest_gtest.sh LinkedListTest.InsertException</t>
+  </si>
+  <si>
+    <t>Run the student main and compare output required output</t>
+  </si>
+  <si>
+    <t>Run cpplint on student code to check coding style</t>
+  </si>
+  <si>
+    <t>Test Method</t>
   </si>
 </sst>
 </file>
@@ -211,11 +221,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,282 +543,476 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D968784-9ABC-434B-B612-3087309D1BAB}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60" customWidth="1"/>
-    <col min="4" max="4" width="68.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="68.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E3:E19)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B4171E-9FB2-AA44-B865-923DD5DD382A}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1">
-        <f>SUM(E3:E19)</f>
+      <c r="C18">
+        <f>SUM(C2:C17)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>